<commit_message>
facut raportu si mai rezolvat de la comentarii
</commit_message>
<xml_diff>
--- a/checklists/Lab01_ReviewReport.xlsx
+++ b/checklists/Lab01_ReviewReport.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="62">
   <si>
     <t xml:space="preserve">do not print this form</t>
   </si>
@@ -75,6 +75,9 @@
     <t xml:space="preserve">Mdaaa, si importul cartilor existente</t>
   </si>
   <si>
+    <t xml:space="preserve">Variable types was not stated</t>
+  </si>
+  <si>
     <t xml:space="preserve">Effort to review document (hours):</t>
   </si>
   <si>
@@ -154,6 +157,57 @@
   </si>
   <si>
     <t xml:space="preserve">Coding Document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CartiRepoMock line 80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se presupune sa ia cartile dintr-un anumit an da le ia alea care nu is in anu ala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validator line 16-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aci tre sa verifice ca lista ii vida, nu nula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some places</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is checking with regex [10-9]+ which is equivalent with [0-9]+ where I presume the desired check would be with 1[0-9]+ (those checks are in the year)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">errors in canfusing function names isOKString and isStringOK, in some places authors were named referents, functiile cautaDupa* din clasa Carte is confuze rau de tot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in repo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">while i&lt;= size should’ve been I &lt; size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in Carte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">an could’ve been integer not string</t>
   </si>
 </sst>
 </file>
@@ -517,7 +571,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -619,14 +673,16 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="13" t="n">
         <f aca="false">B11+1</f>
         <v>3</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
-      <c r="E12" s="15"/>
+      <c r="E12" s="15" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="13" t="n">
@@ -750,7 +806,7 @@
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="14"/>
@@ -781,7 +837,7 @@
   </sheetPr>
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -802,7 +858,7 @@
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -813,13 +869,13 @@
         <v>2</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" s="22"/>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D5" s="23" t="s">
         <v>5</v>
@@ -860,13 +916,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -875,13 +931,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -890,13 +946,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -905,13 +961,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -920,13 +976,13 @@
         <v>5</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -935,13 +991,13 @@
         <v>6</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -950,13 +1006,13 @@
         <v>7</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -965,13 +1021,13 @@
         <v>8</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -980,13 +1036,13 @@
         <v>9</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -995,13 +1051,13 @@
         <v>10</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1072,7 +1128,7 @@
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D28" s="20"/>
       <c r="E28" s="14"/>
@@ -1103,8 +1159,8 @@
   </sheetPr>
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1125,7 +1181,7 @@
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -1139,7 +1195,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E4" s="26"/>
     </row>
@@ -1185,63 +1241,105 @@
       <c r="B10" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="C10" s="0"/>
-      <c r="D10" s="0"/>
-      <c r="E10" s="0"/>
+      <c r="C10" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="13" t="n">
         <f aca="false">B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="0"/>
-      <c r="D11" s="0"/>
-      <c r="E11" s="0"/>
+      <c r="C11" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="13" t="n">
         <f aca="false">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="0"/>
-      <c r="D12" s="0"/>
-      <c r="E12" s="0"/>
-    </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="13" t="n">
         <f aca="false">B12+1</f>
         <v>4</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-    </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="13" t="n">
         <f aca="false">B13+1</f>
         <v>5</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-    </row>
-    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="13" t="n">
         <f aca="false">B14+1</f>
         <v>6</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="13" t="n">
         <f aca="false">B15+1</f>
         <v>7</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
+      <c r="C16" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="13" t="n">
@@ -1374,7 +1472,7 @@
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D32" s="20"/>
       <c r="E32" s="14"/>

</xml_diff>

<commit_message>
rezolvat si codu, practic am facut lab 1
</commit_message>
<xml_diff>
--- a/checklists/Lab01_ReviewReport.xlsx
+++ b/checklists/Lab01_ReviewReport.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="63">
   <si>
     <t xml:space="preserve">do not print this form</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t xml:space="preserve">an could’ve been integer not string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cauta carte dupa autor de fapt cauta dupa cuvinte cheie</t>
   </si>
 </sst>
 </file>
@@ -217,7 +220,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -288,13 +291,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <i val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -442,10 +438,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -472,6 +464,10 @@
     </xf>
     <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -666,7 +662,7 @@
       <c r="C11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E11" s="15" t="s">
@@ -736,7 +732,7 @@
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
-      <c r="E18" s="17"/>
+      <c r="E18" s="16"/>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="13" t="n">
@@ -745,7 +741,7 @@
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
-      <c r="E19" s="17"/>
+      <c r="E19" s="16"/>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="13" t="n">
@@ -754,7 +750,7 @@
       </c>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
-      <c r="E20" s="17"/>
+      <c r="E20" s="16"/>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="13" t="n">
@@ -763,7 +759,7 @@
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
-      <c r="E21" s="17"/>
+      <c r="E21" s="16"/>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="13" t="n">
@@ -772,7 +768,7 @@
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
-      <c r="E22" s="17"/>
+      <c r="E22" s="16"/>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="13" t="n">
@@ -781,7 +777,7 @@
       </c>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
-      <c r="E23" s="17"/>
+      <c r="E23" s="16"/>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="13" t="n">
@@ -790,7 +786,7 @@
       </c>
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
-      <c r="E24" s="17"/>
+      <c r="E24" s="16"/>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="13" t="n">
@@ -799,16 +795,16 @@
       </c>
       <c r="C25" s="13"/>
       <c r="D25" s="13"/>
-      <c r="E25" s="17"/>
+      <c r="E25" s="16"/>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E26" s="18"/>
+      <c r="E26" s="17"/>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="19" t="s">
+      <c r="C27" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="20"/>
+      <c r="D27" s="19"/>
       <c r="E27" s="14"/>
     </row>
   </sheetData>
@@ -865,22 +861,22 @@
       <c r="E2" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="22"/>
+      <c r="E4" s="21"/>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="23"/>
+      <c r="E5" s="22"/>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="8"/>
@@ -915,10 +911,10 @@
       <c r="B10" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E10" s="24" t="s">
@@ -930,10 +926,10 @@
         <f aca="false">B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E11" s="15" t="s">
@@ -945,10 +941,10 @@
         <f aca="false">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E12" s="15" t="s">
@@ -960,10 +956,10 @@
         <f aca="false">B12+1</f>
         <v>4</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E13" s="15" t="s">
@@ -975,10 +971,10 @@
         <f aca="false">B13+1</f>
         <v>5</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E14" s="15" t="s">
@@ -990,10 +986,10 @@
         <f aca="false">B14+1</f>
         <v>6</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E15" s="15" t="s">
@@ -1005,10 +1001,10 @@
         <f aca="false">B15+1</f>
         <v>7</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E16" s="15" t="s">
@@ -1020,10 +1016,10 @@
         <f aca="false">B16+1</f>
         <v>8</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E17" s="15" t="s">
@@ -1035,10 +1031,10 @@
         <f aca="false">B17+1</f>
         <v>9</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E18" s="15" t="s">
@@ -1050,10 +1046,10 @@
         <f aca="false">B18+1</f>
         <v>10</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E19" s="15" t="s">
@@ -1124,13 +1120,13 @@
       <c r="E26" s="15"/>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E27" s="18"/>
+      <c r="E27" s="17"/>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="19" t="s">
+      <c r="C28" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="20"/>
+      <c r="D28" s="19"/>
       <c r="E28" s="14"/>
     </row>
   </sheetData>
@@ -1160,7 +1156,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1188,7 +1184,7 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F3" s="0"/>
+      <c r="F3" s="23"/>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="25" t="s">
@@ -1241,13 +1237,13 @@
       <c r="B10" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="23" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1256,13 +1252,13 @@
         <f aca="false">B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="23" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1271,13 +1267,13 @@
         <f aca="false">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="23" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1341,14 +1337,20 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="13" t="n">
         <f aca="false">B16+1</f>
         <v>8</v>
       </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
+      <c r="C17" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="13" t="n">
@@ -1468,13 +1470,13 @@
       <c r="E30" s="15"/>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E31" s="18"/>
+      <c r="E31" s="17"/>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="19" t="s">
+      <c r="C32" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D32" s="20"/>
+      <c r="D32" s="19"/>
       <c r="E32" s="14"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Asa predau lab 1
</commit_message>
<xml_diff>
--- a/checklists/Lab01_ReviewReport.xlsx
+++ b/checklists/Lab01_ReviewReport.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="68">
   <si>
     <t xml:space="preserve">do not print this form</t>
   </si>
@@ -66,7 +66,7 @@
     <t xml:space="preserve">Proiect 1 Biblioteca</t>
   </si>
   <si>
-    <t xml:space="preserve">Comments: Din ce fisiere vor fi preluate informatiile? Ce format au fisierele? Ce fel de interfata va avea programul? Ce beneficiu am daca ii fac acest program bibliotecii?</t>
+    <t xml:space="preserve">Comments: Din ce fisiere vor fi preluate informatiile? Cand vor fi preluate? Cand se vor specifica fisierele? Ce format au fisierele? Ce fel de interfata va avea programul?  Ce beneficiu am daca ii fac acest program bibliotecii? </t>
   </si>
   <si>
     <t xml:space="preserve">R04</t>
@@ -78,6 +78,12 @@
     <t xml:space="preserve">Variable types was not stated</t>
   </si>
   <si>
+    <t xml:space="preserve">R05, R06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La adaugarea cartilor scrise de un autor, doar de autorul ala sau acel autor sa fie printre autori?</t>
+  </si>
+  <si>
     <t xml:space="preserve">Effort to review document (hours):</t>
   </si>
   <si>
@@ -108,7 +114,7 @@
     <t xml:space="preserve">A03</t>
   </si>
   <si>
-    <t xml:space="preserve">no(see above)</t>
+    <t xml:space="preserve">Campul “editura” nu exista in clasa carte</t>
   </si>
   <si>
     <t xml:space="preserve">A04</t>
@@ -177,6 +183,15 @@
     <t xml:space="preserve">C02</t>
   </si>
   <si>
+    <t xml:space="preserve">C04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CartiRepo line 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File path is wrong</t>
+  </si>
+  <si>
     <t xml:space="preserve">C06</t>
   </si>
   <si>
@@ -210,7 +225,7 @@
     <t xml:space="preserve">an could’ve been integer not string</t>
   </si>
   <si>
-    <t xml:space="preserve">cauta carte dupa autor de fapt cauta dupa cuvinte cheie</t>
+    <t xml:space="preserve">cauta carte dupa autor de fapt cauta dupa cuvinte referenti(aka autorii se numesc referenti)</t>
   </si>
 </sst>
 </file>
@@ -566,8 +581,8 @@
   </sheetPr>
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -640,7 +655,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="13" t="n">
         <v>1</v>
       </c>
@@ -680,14 +695,20 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="13" t="n">
         <f aca="false">B12+1</f>
         <v>4</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="15"/>
+      <c r="C13" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="13" t="n">
@@ -802,7 +823,7 @@
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="18" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D27" s="19"/>
       <c r="E27" s="14"/>
@@ -833,8 +854,8 @@
   </sheetPr>
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -854,7 +875,7 @@
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -865,13 +886,13 @@
         <v>2</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E4" s="21"/>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="20" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D5" s="22" t="s">
         <v>5</v>
@@ -912,13 +933,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -927,139 +948,136 @@
         <v>2</v>
       </c>
       <c r="C11" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="23" t="s">
-        <v>23</v>
-      </c>
       <c r="E11" s="15" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="13" t="n">
-        <f aca="false">B11+1</f>
-        <v>3</v>
-      </c>
+      <c r="B12" s="13"/>
       <c r="C12" s="23" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="13" t="n">
         <f aca="false">B12+1</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="13" t="n">
         <f aca="false">B13+1</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="13" t="n">
         <f aca="false">B14+1</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="13" t="n">
         <f aca="false">B15+1</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="13" t="n">
         <f aca="false">B16+1</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="13" t="n">
         <f aca="false">B17+1</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="13" t="n">
         <f aca="false">B18+1</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="13" t="n">
         <f aca="false">B19+1</f>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
@@ -1068,7 +1086,7 @@
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="13" t="n">
         <f aca="false">B20+1</f>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
@@ -1077,7 +1095,7 @@
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="13" t="n">
         <f aca="false">B21+1</f>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
@@ -1086,7 +1104,7 @@
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="13" t="n">
         <f aca="false">B22+1</f>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>
@@ -1095,7 +1113,7 @@
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="13" t="n">
         <f aca="false">B23+1</f>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C24" s="14"/>
       <c r="D24" s="14"/>
@@ -1104,7 +1122,7 @@
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="13" t="n">
         <f aca="false">B24+1</f>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
@@ -1113,7 +1131,7 @@
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="13" t="n">
         <f aca="false">B25+1</f>
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
@@ -1124,7 +1142,7 @@
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="18" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D28" s="19"/>
       <c r="E28" s="14"/>
@@ -1153,10 +1171,10 @@
     <tabColor rgb="FF8EB4E3"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1177,7 +1195,7 @@
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -1191,7 +1209,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E4" s="26"/>
     </row>
@@ -1238,13 +1256,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1253,13 +1271,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1268,139 +1286,142 @@
         <v>3</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="13" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="13"/>
+      <c r="C13" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="13" t="n">
         <f aca="false">B12+1</f>
         <v>4</v>
       </c>
-      <c r="C13" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="13" t="n">
-        <f aca="false">B13+1</f>
-        <v>5</v>
-      </c>
       <c r="C14" s="14" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="13" t="n">
         <f aca="false">B14+1</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>57</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="13" t="n">
         <f aca="false">B15+1</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="13" t="n">
         <f aca="false">B16+1</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="13" t="n">
         <f aca="false">B17+1</f>
-        <v>9</v>
-      </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
+        <v>8</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="13" t="n">
         <f aca="false">B18+1</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
+      <c r="D19" s="15"/>
       <c r="E19" s="15"/>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="13" t="n">
         <f aca="false">B19+1</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20" s="14"/>
-      <c r="D20" s="15"/>
+      <c r="D20" s="14"/>
       <c r="E20" s="15"/>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="13" t="n">
         <f aca="false">B20+1</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
+      <c r="D21" s="15"/>
       <c r="E21" s="15"/>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="13" t="n">
         <f aca="false">B21+1</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C22" s="14"/>
-      <c r="D22" s="15"/>
+      <c r="D22" s="14"/>
       <c r="E22" s="15"/>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="13" t="n">
         <f aca="false">B22+1</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C23" s="14"/>
       <c r="D23" s="15"/>
@@ -1409,7 +1430,7 @@
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="13" t="n">
         <f aca="false">B23+1</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C24" s="14"/>
       <c r="D24" s="15"/>
@@ -1418,7 +1439,7 @@
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="13" t="n">
         <f aca="false">B24+1</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C25" s="14"/>
       <c r="D25" s="15"/>
@@ -1427,34 +1448,34 @@
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="13" t="n">
         <f aca="false">B25+1</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
+      <c r="D26" s="15"/>
       <c r="E26" s="15"/>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="13" t="n">
         <f aca="false">B26+1</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C27" s="14"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="15"/>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="13" t="n">
         <f aca="false">B27+1</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C28" s="14"/>
       <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
+      <c r="E28" s="14"/>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="13" t="n">
         <f aca="false">B28+1</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C29" s="14"/>
       <c r="D29" s="15"/>
@@ -1463,21 +1484,30 @@
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="13" t="n">
         <f aca="false">B29+1</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C30" s="14"/>
       <c r="D30" s="15"/>
       <c r="E30" s="15"/>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E31" s="17"/>
+      <c r="B31" s="13" t="n">
+        <f aca="false">B30+1</f>
+        <v>21</v>
+      </c>
+      <c r="C31" s="14"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D32" s="19"/>
-      <c r="E32" s="14"/>
+      <c r="E32" s="17"/>
+    </row>
+    <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" s="19"/>
+      <c r="E33" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
am modificat la arhitectura
</commit_message>
<xml_diff>
--- a/checklists/Lab01_ReviewReport.xlsx
+++ b/checklists/Lab01_ReviewReport.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="72">
   <si>
     <t xml:space="preserve">do not print this form</t>
   </si>
@@ -102,13 +102,13 @@
     <t xml:space="preserve">Diagram Biblioteca</t>
   </si>
   <si>
-    <t xml:space="preserve">BibliotecaCtrl: ce cauta acol modifica carte  si sterge carte? Unde ii cautarea dupa autor? CartiRepo: ce cauta acol toate functiile ce trebuiau sa fie in controller si unde is functiile de baza a unui repo? Iara la carti repo, cum dau fisieru? Validator nu o fost specificat in requirements. Carte: constructorul nu are parametrii. Operatii cu referenti si cuvinte cheie care nush ce cauta acolo. Cautarile iara nu au ce cauta acolo. Parsarea din string n-o fost specificata nicaria.</t>
+    <t xml:space="preserve">BibliotecaCtrl: ce cauta acol modifica carte  si sterge carte? CartiRepo: ce cauta acol toate functiile ce trebuiau sa fie in controller si unde is functiile de baza a unui repo? Validator nu o fost specificat in requirements. Carte: constructorul nu are parametrii. Operatii cu referenti si cuvinte cheie care nush ce cauta acolo. Cautarile iara nu au ce cauta acolo. Parsarea din string n-o fost specificata nicaria. </t>
   </si>
   <si>
     <t xml:space="preserve">A02</t>
   </si>
   <si>
-    <t xml:space="preserve">no, separate shit better and don’t add unneeded stuff(see above)</t>
+    <t xml:space="preserve">no, separate things better and don’t add unneeded stuff(see above)</t>
   </si>
   <si>
     <t xml:space="preserve">A03</t>
@@ -132,13 +132,13 @@
     <t xml:space="preserve">A06</t>
   </si>
   <si>
-    <t xml:space="preserve">well, there is inversion of controll, but that’s it</t>
+    <t xml:space="preserve">well, there is inversion of control, but that’s it</t>
   </si>
   <si>
     <t xml:space="preserve">A07</t>
   </si>
   <si>
-    <t xml:space="preserve">“consola” is not clear, would be better named “ui” or something</t>
+    <t xml:space="preserve">“Consola” is not clear, would be better named “UIConsola” or something</t>
   </si>
   <si>
     <t xml:space="preserve">A08</t>
@@ -157,6 +157,18 @@
   </si>
   <si>
     <t xml:space="preserve">what business model? What domain model? See 1 for requirements.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adaugat editura la carte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scos modifica si sterge carte din controller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scos functiile irelevante din repository si le-am pus in controller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scos functiile de cautare dupa autor si cuvinte cheie din Carte</t>
   </si>
   <si>
     <t xml:space="preserve">Review Form. Coding Defects</t>
@@ -854,8 +866,8 @@
   </sheetPr>
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -928,7 +940,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="13" t="n">
         <v>1</v>
       </c>
@@ -1074,50 +1086,58 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="13" t="n">
         <f aca="false">B19+1</f>
         <v>8</v>
       </c>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
-      <c r="E20" s="15"/>
-    </row>
-    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E20" s="0"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="13" t="n">
         <f aca="false">B20+1</f>
         <v>9</v>
       </c>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
-      <c r="E21" s="15"/>
-    </row>
-    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E21" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="13" t="n">
         <f aca="false">B21+1</f>
         <v>10</v>
       </c>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
-      <c r="E22" s="15"/>
-    </row>
-    <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E22" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="13" t="n">
         <f aca="false">B22+1</f>
         <v>11</v>
       </c>
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>
-      <c r="E23" s="15"/>
-    </row>
-    <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E23" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="13" t="n">
         <f aca="false">B23+1</f>
         <v>12</v>
       </c>
       <c r="C24" s="14"/>
       <c r="D24" s="14"/>
-      <c r="E24" s="15"/>
+      <c r="E24" s="15" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="13" t="n">
@@ -1173,8 +1193,8 @@
   </sheetPr>
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1195,7 +1215,7 @@
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -1209,7 +1229,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E4" s="26"/>
     </row>
@@ -1256,13 +1276,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1271,13 +1291,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1286,25 +1306,25 @@
         <v>3</v>
       </c>
       <c r="C12" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="23" t="s">
-        <v>48</v>
-      </c>
       <c r="E12" s="23" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="13"/>
       <c r="C13" s="23" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1313,13 +1333,13 @@
         <v>4</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1328,13 +1348,13 @@
         <v>5</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1343,13 +1363,13 @@
         <v>6</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1358,13 +1378,13 @@
         <v>7</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1373,13 +1393,13 @@
         <v>8</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>